<commit_message>
feat: add final code
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/darmawan/work/gyh/Analysis/rula-analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{787B375E-5E01-E944-82BA-E4B15FB31E8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB76AF74-EA9F-7640-B244-4FEE6690CFC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -450,7 +450,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -521,10 +521,10 @@
         <v>16</v>
       </c>
       <c r="C2" s="2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D2" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E2" s="2">
         <v>2</v>
@@ -562,7 +562,7 @@
         <v>17</v>
       </c>
       <c r="C3" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D3" s="2">
         <v>2</v>
@@ -583,7 +583,7 @@
         <v>1</v>
       </c>
       <c r="J3" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K3" s="2">
         <v>2</v>
@@ -603,34 +603,34 @@
         <v>18</v>
       </c>
       <c r="C4" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D4" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F4" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G4" s="2">
         <v>1</v>
       </c>
       <c r="H4" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I4" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J4" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K4" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L4" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M4" s="2">
         <v>1</v>

</xml_diff>